<commit_message>
Change-Id: I8ef333eb8bfb83b42081718d20aecc495ac4c8ce Signed-off-by: Eason.ZHANG <zhyj663@163.com>
</commit_message>
<xml_diff>
--- a/dat/test case.xlsx
+++ b/dat/test case.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>prefer</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,6 +52,30 @@
   </si>
   <si>
     <t>poolname</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>www</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ty</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -396,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -445,6 +469,36 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -456,10 +510,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Change-Id: I974c538cfa931a5d138bc21b83276e2467053b17 Signed-off-by: Eason.ZHANG <zhyj663@163.com>
</commit_message>
<xml_diff>
--- a/dat/test case.xlsx
+++ b/dat/test case.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>prefer</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,47 +59,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>板块轮动策略</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>e</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>d</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>t</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>的</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对</t>
+    <t>板块热点轮动策略</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -444,13 +404,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="15.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -493,61 +457,6 @@
       </c>
       <c r="C2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>